<commit_message>
Regretion Run SCD0011 - Produk Detail, SCD0012 - Upload List File, SCD0013 - Upload List File, SCD0014 - Upload List File
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0011_Produk Detail.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0011_Produk Detail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01A2B1D-3692-4658-8C70-60AE77D6E5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67020A0F-B9F2-4AA5-A697-C76822EE7CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>SIDEBAR_SUBMENU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>SIDEBAR_SUBMENU_SUBMENU</t>
   </si>
@@ -74,6 +71,12 @@
   </si>
   <si>
     <t>Muncul pop up Berhasil mengirim link</t>
+  </si>
+  <si>
+    <t>SUB_NAVBAR</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
   </si>
 </sst>
 </file>
@@ -474,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.7109375" customWidth="1"/>
     <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
@@ -503,68 +506,70 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
         <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="12">
         <v>55210</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K2" s="7"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>

</xml_diff>